<commit_message>
update to wrk with miniconda py38
</commit_message>
<xml_diff>
--- a/notebookccdm_gen3/runspectractor_standalone/2023_07/logbooks/auxtellogbook_empty~holo4_003_20230119_v6.0.xlsx
+++ b/notebookccdm_gen3/runspectractor_standalone/2023_07/logbooks/auxtellogbook_empty~holo4_003_20230119_v6.0.xlsx
@@ -564,7 +564,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -640,7 +640,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -792,7 +792,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -868,7 +868,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -944,7 +944,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1248,7 +1248,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1476,7 +1476,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1704,7 +1704,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1932,7 +1932,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2084,7 +2084,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -2160,7 +2160,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2388,7 +2388,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -2464,7 +2464,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -2616,7 +2616,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -2844,7 +2844,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -2920,7 +2920,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -2996,7 +2996,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -3072,7 +3072,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -3148,7 +3148,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -3224,7 +3224,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -3300,7 +3300,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -3376,7 +3376,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -3528,7 +3528,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -3680,7 +3680,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -3756,7 +3756,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>/Users/sylvie/DATA/AuxTelData2023/data/2023/empty~holo4_003/20230119</t>
+          <t>/sps/lsst/groups/auxtel/data/hack_usdf/my_postisrccd_img_forspectractor_2023/empty~holo4_003/20230119</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">

</xml_diff>